<commit_message>
Updated with projected completion dates
</commit_message>
<xml_diff>
--- a/Example Database.xlsx
+++ b/Example Database.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="143">
   <si>
     <t>Users</t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t>Week</t>
+  </si>
+  <si>
+    <t>Completed goal</t>
   </si>
   <si>
     <t>User control</t>
@@ -446,10 +449,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm"/>
     <numFmt numFmtId="166" formatCode="m-d"/>
+    <numFmt numFmtId="167" formatCode="m/d"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -563,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -685,6 +689,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -2322,60 +2329,78 @@
       <c r="C1" s="8" t="s">
         <v>131</v>
       </c>
+      <c r="D1" s="23" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C2" s="47">
         <v>44960.0</v>
       </c>
+      <c r="D2" s="48">
+        <v>45245.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="48">
+        <v>136</v>
+      </c>
+      <c r="C3" s="49">
         <v>4.0</v>
+      </c>
+      <c r="D3" s="48">
+        <v>45252.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="48">
-        <v>1.0</v>
+        <v>138</v>
+      </c>
+      <c r="C4" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="48">
+        <v>45231.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="48">
+        <v>140</v>
+      </c>
+      <c r="C5" s="49">
         <v>4.0</v>
+      </c>
+      <c r="D5" s="48">
+        <v>45252.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="C6" s="48">
-        <v>1.0</v>
+        <v>142</v>
+      </c>
+      <c r="C6" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="48">
+        <v>45231.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>